<commit_message>
Allocation Web link Asset Web
</commit_message>
<xml_diff>
--- a/File/Mẫu nhập tài sản đã cấp phát (2).xlsx
+++ b/File/Mẫu nhập tài sản đã cấp phát (2).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tester\Auto\Selenium\Login\File\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\asset\asset-maintenance\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B107761-C96B-4BD6-B3A1-2701EDF7CA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AD576D-3F05-4C40-8858-22F311E101B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ds cấp phát TSCĐ" sheetId="2" r:id="rId1"/>
@@ -23,9 +23,9 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{F1B5133D-73B0-46B4-AACD-A8D062B66C90}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{FCBE8BD3-6A36-495B-A83B-5AA96605B849}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{5897698B-E59D-42B0-A575-7C1ECF9C3848}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{FCBE8BD3-6A36-495B-A83B-5AA96605B849}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{F1B5133D-73B0-46B4-AACD-A8D062B66C90}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>ma_phong_ban</t>
   </si>
@@ -224,46 +224,37 @@
     <t>1</t>
   </si>
   <si>
-    <t>TS-008496</t>
-  </si>
-  <si>
-    <t>TSM</t>
-  </si>
-  <si>
-    <t>26/04/2025</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>TS-007876</t>
-  </si>
-  <si>
-    <t>KT001</t>
-  </si>
-  <si>
-    <t>4.3.KXN</t>
-  </si>
-  <si>
-    <t>27/11/2024</t>
-  </si>
-  <si>
-    <t>29/02/2025</t>
-  </si>
-  <si>
-    <t>bv199</t>
-  </si>
-  <si>
-    <t>26/11/2024</t>
-  </si>
-  <si>
-    <t>TS-007871</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mã tài sản bị trống.</t>
-  </si>
-  <si>
-    <t>Errors</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>TS-001630</t>
+  </si>
+  <si>
+    <t>TS-001629</t>
+  </si>
+  <si>
+    <t>30/03/2024</t>
+  </si>
+  <si>
+    <t>02/04/2024</t>
+  </si>
+  <si>
+    <t>KM</t>
+  </si>
+  <si>
+    <t>5.KN</t>
+  </si>
+  <si>
+    <t>longau</t>
+  </si>
+  <si>
+    <t>pgd1</t>
+  </si>
+  <si>
+    <t>Ghi chú 1</t>
+  </si>
+  <si>
+    <t>Ghi chú 2</t>
   </si>
 </sst>
 </file>
@@ -271,7 +262,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -338,13 +329,8 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,23 +353,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF0000"/>
-        <bgColor rgb="FF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0000"/>
-        <bgColor rgb="FF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -475,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -546,7 +515,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,25 +733,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A8" sqref="A8:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="15" width="5.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="15" width="21.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="14" width="27.88671875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="23" width="26.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="14" width="26.21875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="14" width="23.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="14" width="28.21875" collapsed="true"/>
-    <col min="8" max="16384" style="14" width="12.77734375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="15" width="5.46484375" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="15" width="21.46484375" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="14" width="27.86328125" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="23" width="26.46484375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="14" width="26.19921875" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="14" width="23.86328125" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="14" width="28.19921875" collapsed="false"/>
+    <col min="8" max="16384" style="14" width="12.796875" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="24" t="s">
         <v>42</v>
       </c>
@@ -794,7 +762,7 @@
       <c r="F1" s="24"/>
       <c r="G1" s="24"/>
     </row>
-    <row r="2" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -803,7 +771,7 @@
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
     </row>
-    <row r="3" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="13" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="25" t="s">
         <v>41</v>
       </c>
@@ -814,7 +782,7 @@
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
     </row>
-    <row r="4" spans="1:7" s="12" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="12" customFormat="1" ht="13.5" x14ac:dyDescent="0.45">
       <c r="A4" s="16" t="s">
         <v>30</v>
       </c>
@@ -836,11 +804,8 @@
       <c r="G4" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="H4" t="s" s="28">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="18" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" s="18" customFormat="1" ht="41.65" x14ac:dyDescent="0.45">
       <c r="A5" s="19"/>
       <c r="B5" s="20" t="s">
         <v>37</v>
@@ -861,31 +826,75 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s" s="15">
+    <row r="6" spans="1:7" ht="13.9" x14ac:dyDescent="0.45">
+      <c r="A6" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B6" t="s" s="15">
+      <c r="B6" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="13.9" x14ac:dyDescent="0.45">
+      <c r="A7" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C6" t="s" s="14">
-        <v>49</v>
-      </c>
-      <c r="D6" t="s" s="23">
-        <v>51</v>
-      </c>
-      <c r="E6" t="s" s="14">
-        <v>52</v>
-      </c>
-      <c r="H6" t="s">
-        <v>58</v>
+      <c r="G7" s="14" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{5897698B-E59D-42B0-A575-7C1ECF9C3848}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:Y254" xr:uid="{4ED84E6D-B3A9-46C5-8D33-B68DBD154420}"/>
+      <extLst>
+        <ext uri="GoogleSheetsCustomDataVersion1">
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1416023640"/>
+        </ext>
+      </extLst>
+    </customSheetView>
+    <customSheetView guid="{F1B5133D-73B0-46B4-AACD-A8D062B66C90}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A2:Y1126" xr:uid="{386DF583-C0A4-4A2E-8228-62A6C1C0A67D}"/>
+      <extLst>
+        <ext uri="GoogleSheetsCustomDataVersion1">
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1669903916"/>
+        </ext>
+      </extLst>
+    </customSheetView>
     <customSheetView guid="{FCBE8BD3-6A36-495B-A83B-5AA96605B849}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:Z1377" xr:uid="{7BFA42ED-B847-464B-9B73-5549640F2AF9}">
+      <autoFilter ref="A2:Z1377" xr:uid="{941047CB-87F9-4B8E-A3AD-79EDC147B9BB}">
         <filterColumn colId="4">
           <filters>
             <filter val="- 02Hệ tủ tài liệu treo tường , 03 Bàn làm việc, Bộ Salon Thẳng, Bàn trà kính"/>
@@ -922,24 +931,6 @@
         </ext>
       </extLst>
     </customSheetView>
-    <customSheetView guid="{F1B5133D-73B0-46B4-AACD-A8D062B66C90}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:Y1126" xr:uid="{C45E7315-58EF-4595-8566-41135570AC78}"/>
-      <extLst>
-        <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1669903916"/>
-        </ext>
-      </extLst>
-    </customSheetView>
-    <customSheetView guid="{5897698B-E59D-42B0-A575-7C1ECF9C3848}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:Y254" xr:uid="{003304EE-EB25-485D-AD7D-22B184DFC7C9}"/>
-      <extLst>
-        <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1416023640"/>
-        </ext>
-      </extLst>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
     <mergeCell ref="A1:G1"/>
@@ -959,12 +950,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="40.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="40.0" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -984,7 +975,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -999,7 +990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>18</v>
       </c>
@@ -1016,7 +1007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>20</v>
       </c>
@@ -1030,7 +1021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
         <v>22</v>
       </c>
@@ -1044,7 +1035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>24</v>
       </c>
@@ -1061,7 +1052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
@@ -1079,7 +1070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
         <v>15</v>
       </c>
@@ -1093,7 +1084,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
         <v>12</v>
       </c>
@@ -1113,7 +1104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
         <v>13</v>
       </c>
@@ -1130,7 +1121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
         <v>14</v>
       </c>
@@ -1147,7 +1138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
         <v>29</v>
       </c>

</xml_diff>